<commit_message>
+ fremde daten :)
</commit_message>
<xml_diff>
--- a/LIL/Data/Auswertung.xlsx
+++ b/LIL/Data/Auswertung.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="242" yWindow="100" windowWidth="14799" windowHeight="8013" activeTab="2"/>
+    <workbookView xWindow="242" yWindow="100" windowWidth="14799" windowHeight="8013"/>
   </bookViews>
   <sheets>
-    <sheet name="80 mJ" sheetId="1" r:id="rId1"/>
-    <sheet name="120 mJ" sheetId="2" r:id="rId2"/>
-    <sheet name="160 mJ" sheetId="3" r:id="rId3"/>
+    <sheet name="10 mJ" sheetId="4" r:id="rId1"/>
+    <sheet name="40 mJ" sheetId="5" r:id="rId2"/>
+    <sheet name="80 mJ" sheetId="1" r:id="rId3"/>
+    <sheet name="120 mJ" sheetId="2" r:id="rId4"/>
+    <sheet name="160 mJ" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="7">
   <si>
     <t>Amplituden</t>
   </si>
@@ -34,6 +36,9 @@
   </si>
   <si>
     <t>StdAbweichung</t>
+  </si>
+  <si>
+    <t>--</t>
   </si>
 </sst>
 </file>
@@ -69,8 +74,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -374,8 +380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -385,14 +391,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
+      <c r="A1">
+        <v>10</v>
+      </c>
+      <c r="B1">
+        <v>20</v>
+      </c>
+      <c r="C1">
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -402,56 +408,63 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>49.526000000000003</v>
+        <v>79</v>
       </c>
       <c r="B3">
-        <v>43.427</v>
-      </c>
-      <c r="C3">
-        <v>75.302000000000007</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>47.875</v>
+        <v>125</v>
       </c>
       <c r="B4">
-        <v>40.082000000000001</v>
+        <v>118</v>
       </c>
       <c r="C4">
-        <v>75.656999999999996</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>34.095999999999997</v>
+        <v>149</v>
       </c>
       <c r="B5">
-        <v>38.613999999999997</v>
+        <v>108</v>
       </c>
       <c r="C5">
-        <v>66.676000000000002</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>38.164000000000001</v>
+        <v>116</v>
       </c>
       <c r="B6">
-        <v>32.475000000000001</v>
+        <v>125</v>
       </c>
       <c r="C6">
-        <v>63.890999999999998</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>160</v>
+      </c>
       <c r="B7">
-        <v>33.377000000000002</v>
+        <v>128</v>
+      </c>
+      <c r="C7">
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8">
-        <v>32.545000000000002</v>
+        <v>111</v>
+      </c>
+      <c r="C8">
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -462,6 +475,311 @@
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <f>AVERAGE(A3:A10)</f>
+        <v>125.8</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ref="B14:C14" si="0">AVERAGE(B3:B10)</f>
+        <v>116.5</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>93.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f>STDEVA(A3:A8)</f>
+        <v>31.60221511223542</v>
+      </c>
+      <c r="B17">
+        <f t="shared" ref="B17:C17" si="1">STDEVA(B3:B8)</f>
+        <v>8.5498537999196209</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>7.8230428862431785</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>10</v>
+      </c>
+      <c r="B1">
+        <v>20</v>
+      </c>
+      <c r="C1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>78</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>79</v>
+      </c>
+      <c r="B4">
+        <v>117</v>
+      </c>
+      <c r="C4">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>74</v>
+      </c>
+      <c r="B5">
+        <v>124</v>
+      </c>
+      <c r="C5">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>87</v>
+      </c>
+      <c r="B6">
+        <v>122</v>
+      </c>
+      <c r="C6">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>82</v>
+      </c>
+      <c r="B7">
+        <v>128</v>
+      </c>
+      <c r="C7">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>88</v>
+      </c>
+      <c r="C8">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f>AVERAGE(A3:A10)</f>
+        <v>81.333333333333329</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ref="B14:C14" si="0">AVERAGE(B3:B10)</f>
+        <v>122.75</v>
+      </c>
+      <c r="C14">
+        <f>AVERAGE(C3:C10)</f>
+        <v>66.833333333333329</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f>STDEVA(A3:A8)</f>
+        <v>5.4283207962192757</v>
+      </c>
+      <c r="B17">
+        <f t="shared" ref="B17:C17" si="1">STDEVA(B3:B8)</f>
+        <v>55.038168574181327</v>
+      </c>
+      <c r="C17">
+        <f>STDEVA(C3:C8)</f>
+        <v>8.4715209181507909</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1">
+        <v>20</v>
+      </c>
+      <c r="E1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>49.526000000000003</v>
+      </c>
+      <c r="B3">
+        <v>43.427</v>
+      </c>
+      <c r="C3">
+        <v>75.302000000000007</v>
+      </c>
+      <c r="D3">
+        <v>66</v>
+      </c>
+      <c r="E3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>47.875</v>
+      </c>
+      <c r="B4">
+        <v>40.082000000000001</v>
+      </c>
+      <c r="C4">
+        <v>75.656999999999996</v>
+      </c>
+      <c r="D4">
+        <v>72</v>
+      </c>
+      <c r="E4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>34.095999999999997</v>
+      </c>
+      <c r="B5">
+        <v>38.613999999999997</v>
+      </c>
+      <c r="C5">
+        <v>66.676000000000002</v>
+      </c>
+      <c r="D5">
+        <v>66</v>
+      </c>
+      <c r="E5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>38.164000000000001</v>
+      </c>
+      <c r="B6">
+        <v>32.475000000000001</v>
+      </c>
+      <c r="C6">
+        <v>63.890999999999998</v>
+      </c>
+      <c r="D6">
+        <v>77</v>
+      </c>
+      <c r="E6">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>33.377000000000002</v>
+      </c>
+      <c r="D7">
+        <v>81</v>
+      </c>
+      <c r="E7">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>32.545000000000002</v>
+      </c>
+      <c r="D8">
+        <v>74</v>
+      </c>
+      <c r="E8">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f>AVERAGE(A3:A10)</f>
         <v>42.41525</v>
       </c>
       <c r="B14">
@@ -472,24 +790,40 @@
         <f t="shared" si="0"/>
         <v>70.381500000000003</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <f t="shared" ref="D14:E14" si="1">AVERAGE(D3:D10)</f>
+        <v>72.666666666666671</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>24.666666666666668</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <f>STDEVA(A3:A8)</f>
         <v>7.4756199910107712</v>
       </c>
       <c r="B17">
-        <f t="shared" ref="B17:C17" si="1">STDEVA(B3:B8)</f>
+        <f t="shared" ref="B17:C17" si="2">STDEVA(B3:B8)</f>
         <v>4.615057124962485</v>
       </c>
       <c r="C17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.9972088229998031</v>
+      </c>
+      <c r="D17">
+        <f t="shared" ref="D17:E17" si="3">STDEVA(D3:D8)</f>
+        <v>5.9888785817268548</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="3"/>
+        <v>5.2788887719544437</v>
       </c>
     </row>
   </sheetData>
@@ -497,7 +831,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
@@ -596,12 +930,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D37" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>

</xml_diff>